<commit_message>
adding means and plots
</commit_message>
<xml_diff>
--- a/other/Embedded_Features.xlsx
+++ b/other/Embedded_Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cv/dsi/capstones/cap_3/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DB7D7A-FE64-3949-838B-5D330A3743B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0707A5E-DD86-664F-A607-466947091AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="620" windowWidth="27640" windowHeight="16220" xr2:uid="{FD636BD8-387D-7C4A-9332-BE1A6A12FDD6}"/>
+    <workbookView xWindow="30720" yWindow="2100" windowWidth="21260" windowHeight="13940" xr2:uid="{FD636BD8-387D-7C4A-9332-BE1A6A12FDD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="236">
   <si>
     <t>oem</t>
   </si>
@@ -646,6 +646,102 @@
   </si>
   <si>
     <t xml:space="preserve"> back</t>
+  </si>
+  <si>
+    <t>UMTS</t>
+  </si>
+  <si>
+    <t>panorama</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> colors</t>
+  </si>
+  <si>
+    <t>touch/touchscreen</t>
+  </si>
+  <si>
+    <t>waterproof/water proof</t>
+  </si>
+  <si>
+    <t>removable</t>
+  </si>
+  <si>
+    <t>non-removable</t>
+  </si>
+  <si>
+    <t>STN</t>
+  </si>
+  <si>
+    <t>CSTN</t>
+  </si>
+  <si>
+    <t>ASV</t>
+  </si>
+  <si>
+    <t>kickstand</t>
+  </si>
+  <si>
+    <t>splah</t>
+  </si>
+  <si>
+    <t>splash</t>
+  </si>
+  <si>
+    <t>dust</t>
+  </si>
+  <si>
+    <t>flashlight</t>
+  </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>pay</t>
+  </si>
+  <si>
+    <t>stylus</t>
+  </si>
+  <si>
+    <t>dual-core</t>
+  </si>
+  <si>
+    <t>quad-core</t>
+  </si>
+  <si>
+    <t>hexa-core</t>
+  </si>
+  <si>
+    <t>octa-core</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>voice</t>
+  </si>
+  <si>
+    <t>reverse</t>
+  </si>
+  <si>
+    <t>fast</t>
+  </si>
+  <si>
+    <t>wireless</t>
+  </si>
+  <si>
+    <t>zoom</t>
+  </si>
+  <si>
+    <t>flash</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>monochrome</t>
+  </si>
+  <si>
+    <t>color</t>
   </si>
 </sst>
 </file>
@@ -661,7 +757,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,6 +767,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,9 +801,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,15 +1124,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E47C21D-0C79-0645-BEC8-466865656912}">
   <dimension ref="A1:CH32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="23" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="20" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="17" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="20" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="15" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:86">
@@ -1039,10 +1238,10 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -1075,7 +1274,7 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="U1" t="s">
@@ -1114,13 +1313,13 @@
       <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" t="s">
@@ -1135,7 +1334,7 @@
       <c r="AM1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="5" t="s">
         <v>39</v>
       </c>
       <c r="AO1" t="s">
@@ -1153,25 +1352,25 @@
       <c r="AS1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AV1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AX1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AY1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>51</v>
       </c>
       <c r="BA1" t="s">
@@ -1180,40 +1379,40 @@
       <c r="BB1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>54</v>
       </c>
       <c r="BD1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BE1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BF1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BG1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BH1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BK1" s="4" t="s">
         <v>62</v>
       </c>
       <c r="BL1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BM1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BN1" s="5" t="s">
         <v>65</v>
       </c>
       <c r="BO1" t="s">
@@ -1222,58 +1421,58 @@
       <c r="BP1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BR1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BS1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BT1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BU1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BV1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BW1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BX1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BY1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>77</v>
       </c>
       <c r="CA1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CB1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CC1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CD1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CE1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CF1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CG1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CH1" s="2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1372,7 +1571,7 @@
         <v>193</v>
       </c>
       <c r="AS2" t="s">
-        <v>189</v>
+        <v>232</v>
       </c>
       <c r="BA2" s="1" t="s">
         <v>195</v>
@@ -1407,7 +1606,7 @@
         <v>95</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>97</v>
+        <v>208</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>101</v>
@@ -1531,6 +1730,15 @@
       <c r="AL4" t="s">
         <v>160</v>
       </c>
+      <c r="AP4" t="s">
+        <v>205</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>226</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>228</v>
+      </c>
       <c r="BL4" s="1" t="s">
         <v>199</v>
       </c>
@@ -1569,11 +1777,17 @@
       <c r="AF5" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="AG5" t="s">
+        <v>209</v>
+      </c>
       <c r="AK5">
         <v>1900</v>
       </c>
       <c r="AL5" t="s">
         <v>161</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>227</v>
       </c>
       <c r="BL5" s="1" t="s">
         <v>200</v>
@@ -1589,6 +1803,12 @@
       <c r="D6" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="L6" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="R6" t="s">
         <v>114</v>
       </c>
@@ -1604,6 +1824,9 @@
       <c r="AF6" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="AG6" t="s">
+        <v>210</v>
+      </c>
       <c r="AK6">
         <v>2100</v>
       </c>
@@ -1618,6 +1841,15 @@
       </c>
     </row>
     <row r="7" spans="1:86">
+      <c r="C7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="AA7" s="1" t="s">
         <v>129</v>
       </c>
@@ -1633,6 +1865,9 @@
       <c r="AL7" t="s">
         <v>163</v>
       </c>
+      <c r="BB7" t="s">
+        <v>229</v>
+      </c>
       <c r="BL7" s="1" t="s">
         <v>202</v>
       </c>
@@ -1641,22 +1876,46 @@
       </c>
     </row>
     <row r="8" spans="1:86">
+      <c r="L8" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="AF8" s="1" t="s">
         <v>148</v>
       </c>
       <c r="AL8" t="s">
         <v>164</v>
       </c>
+      <c r="BB8" t="s">
+        <v>230</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>55</v>
+      </c>
+      <c r="BL8" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="9" spans="1:86">
+      <c r="L9" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="AF9" s="1" t="s">
         <v>151</v>
       </c>
       <c r="AL9" t="s">
         <v>165</v>
       </c>
+      <c r="BB9" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="10" spans="1:86">
+      <c r="M10" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AF10" s="1" t="s">
         <v>149</v>
       </c>
@@ -1665,14 +1924,29 @@
       </c>
     </row>
     <row r="11" spans="1:86">
+      <c r="M11" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="AF11" s="1" t="s">
         <v>150</v>
       </c>
       <c r="AL11" t="s">
         <v>167</v>
       </c>
+      <c r="BL11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:86">
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="AF12" s="1" t="s">
         <v>152</v>
       </c>
@@ -1702,86 +1976,199 @@
       </c>
     </row>
     <row r="16" spans="1:86">
+      <c r="L16" t="s">
+        <v>96</v>
+      </c>
+      <c r="M16" t="s">
+        <v>100</v>
+      </c>
+      <c r="R16" t="s">
+        <v>222</v>
+      </c>
+      <c r="S16" t="s">
+        <v>18</v>
+      </c>
+      <c r="V16" t="s">
+        <v>21</v>
+      </c>
+      <c r="X16" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ16" t="s">
+        <v>35</v>
+      </c>
       <c r="AL16" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="38:38">
+    <row r="17" spans="12:45">
+      <c r="L17" t="s">
+        <v>97</v>
+      </c>
+      <c r="M17" t="s">
+        <v>101</v>
+      </c>
+      <c r="R17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>210</v>
+      </c>
       <c r="AL17" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="18" spans="38:38">
+      <c r="AP17" s="3"/>
+    </row>
+    <row r="18" spans="12:45">
+      <c r="L18" t="s">
+        <v>220</v>
+      </c>
+      <c r="M18" t="s">
+        <v>102</v>
+      </c>
+      <c r="R18" t="s">
+        <v>224</v>
+      </c>
       <c r="AL18" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="19" spans="38:38">
+      <c r="AP18" s="3"/>
+    </row>
+    <row r="19" spans="12:45">
+      <c r="L19" t="s">
+        <v>221</v>
+      </c>
+      <c r="M19" t="s">
+        <v>103</v>
+      </c>
+      <c r="R19" t="s">
+        <v>225</v>
+      </c>
       <c r="AL19" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="20" spans="38:38">
+      <c r="AP19" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="AQ19" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AS19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="12:45">
+      <c r="L20" t="s">
+        <v>214</v>
+      </c>
+      <c r="M20" t="s">
+        <v>207</v>
+      </c>
       <c r="AL20" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="21" spans="38:38">
+      <c r="AP20" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AQ20" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AS20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="12:45">
+      <c r="L21" t="s">
+        <v>215</v>
+      </c>
       <c r="AL21" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="22" spans="38:38">
+      <c r="AP21" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="12:45">
+      <c r="L22" t="s">
+        <v>218</v>
+      </c>
       <c r="AL22" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="23" spans="38:38">
+      <c r="AP22" s="3"/>
+    </row>
+    <row r="23" spans="12:45">
+      <c r="M23" t="s">
+        <v>234</v>
+      </c>
       <c r="AL23" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="24" spans="38:38">
+      <c r="AP23" s="3"/>
+    </row>
+    <row r="24" spans="12:45">
+      <c r="M24" t="s">
+        <v>235</v>
+      </c>
       <c r="AL24" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="25" spans="38:38">
+      <c r="AP24" s="3"/>
+    </row>
+    <row r="25" spans="12:45">
       <c r="AL25" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="26" spans="38:38">
+      <c r="AP25" s="3"/>
+    </row>
+    <row r="26" spans="12:45">
       <c r="AL26" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="27" spans="38:38">
+      <c r="AP26" s="3"/>
+    </row>
+    <row r="27" spans="12:45">
       <c r="AL27">
         <v>46</v>
       </c>
-    </row>
-    <row r="28" spans="38:38">
+      <c r="AP27" s="3"/>
+    </row>
+    <row r="28" spans="12:45">
       <c r="AL28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="38:38">
+    <row r="29" spans="12:45">
       <c r="AL29" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="38:38">
+    <row r="30" spans="12:45">
       <c r="AL30" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="38:38">
+    <row r="31" spans="12:45">
       <c r="AL31" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="32" spans="38:38">
+    <row r="32" spans="12:45">
       <c r="AL32" s="1" t="s">
         <v>115</v>
       </c>

</xml_diff>